<commit_message>
updated linear regression with error chart
</commit_message>
<xml_diff>
--- a/models_in_excel/Linear_Regression.xlsx
+++ b/models_in_excel/Linear_Regression.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Books\AI\Practice\PDF\Karim\EXCEL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Books\AI\Practice\PDF\Karim\EXCEL\Git_hub\ML_Models\models_in_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2595EDBF-2653-4102-BB0A-03814FDCFE6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7875F7F4-E9E8-4FF5-8E79-DEDFA9FC86BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,17 +18,28 @@
     <sheet name="PDF_normalzation" sheetId="1" r:id="rId3"/>
     <sheet name="Linear_Regression" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="34">
   <si>
     <t>price</t>
   </si>
@@ -275,6 +286,12 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>Predicted(Y)</t>
+  </si>
+  <si>
+    <t>Error</t>
   </si>
 </sst>
 </file>
@@ -12359,8 +12376,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95E4E5C9-30C2-46DA-ADDA-91E751A0E456}">
   <dimension ref="B4:P42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5:I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12408,6 +12425,12 @@
       <c r="E5" s="30"/>
       <c r="F5" s="50"/>
       <c r="G5" s="51"/>
+      <c r="H5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="L5" s="59" t="s">
         <v>24</v>
       </c>

</xml_diff>

<commit_message>
updated linear regression with 3 variables
</commit_message>
<xml_diff>
--- a/models_in_excel/Linear_Regression.xlsx
+++ b/models_in_excel/Linear_Regression.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Books\AI\Practice\PDF\Karim\EXCEL\Git_hub\ML_Models\models_in_excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Books\AI\Practice\PDF\Karim\EXCEL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7875F7F4-E9E8-4FF5-8E79-DEDFA9FC86BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B70D9A6E-4A58-4A95-A2E9-9C8EFA553593}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,28 +18,20 @@
     <sheet name="PDF_normalzation" sheetId="1" r:id="rId3"/>
     <sheet name="Linear_Regression" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">Linear_Regression!$F$6:$F$39</definedName>
+  </definedNames>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="25">
   <si>
     <t>price</t>
   </si>
@@ -182,11 +174,21 @@
     <t xml:space="preserve">Variance </t>
   </si>
   <si>
+    <t>=</t>
+  </si>
+  <si>
+    <t>Predicted(y)</t>
+  </si>
+  <si>
+    <t>Error</t>
+  </si>
+  <si>
     <r>
-      <t>X</t>
+      <t>Error</t>
     </r>
     <r>
       <rPr>
+        <b/>
         <vertAlign val="superscript"/>
         <sz val="11"/>
         <color theme="1"/>
@@ -196,102 +198,6 @@
       </rPr>
       <t>2</t>
     </r>
-  </si>
-  <si>
-    <t>SUM=</t>
-  </si>
-  <si>
-    <r>
-      <t>x</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>i</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>*Y</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>i</t>
-    </r>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>=</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <r>
-      <t>a</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>a</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1</t>
-    </r>
-  </si>
-  <si>
-    <t>A^-1</t>
-  </si>
-  <si>
-    <t>x = A^-1*B</t>
-  </si>
-  <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>Predicted(Y)</t>
-  </si>
-  <si>
-    <t>Error</t>
   </si>
 </sst>
 </file>
@@ -371,6 +277,7 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <vertAlign val="superscript"/>
       <sz val="11"/>
       <color theme="1"/>
@@ -399,7 +306,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="27">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -528,21 +435,6 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
       <right/>
       <top style="medium">
         <color indexed="64"/>
@@ -663,37 +555,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -724,49 +590,45 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2840,14 +2702,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.27248379055357808"/>
-          <c:y val="2.4330900243309004E-2"/>
-        </c:manualLayout>
-      </c:layout>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Area Vs Price</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2881,16 +2760,25 @@
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
-        <c:scatterStyle val="smoothMarker"/>
+        <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Linear_Regression!$D$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>price</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
+              <a:noFill/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -2926,8 +2814,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.29331234510320359"/>
-                  <c:y val="-0.30097374719111386"/>
+                  <c:x val="0.21277580927384077"/>
+                  <c:y val="-0.27216899970836977"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -2962,122 +2850,122 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
+              <c:f>Linear_Regression!$C$6:$C$39</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="34"/>
+                <c:pt idx="0">
+                  <c:v>7420</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8960</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7420</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8580</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8100</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5750</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6550</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7800</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6600</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>8500</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4600</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6420</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4320</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>7155</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>8050</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4560</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>8800</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>6540</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>6000</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>8875</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>7950</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>5500</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>7475</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>7000</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>4880</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>5960</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>6840</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>7000</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>7482</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>9000</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>6000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
               <c:f>Linear_Regression!$D$6:$D$39</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="34"/>
                 <c:pt idx="0">
-                  <c:v>7420</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>8960</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>7500</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>7420</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7500</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>8580</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>8100</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>5750</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>6000</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>6550</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>7800</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>6600</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>8500</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>4600</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>6420</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>4320</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>7155</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>8050</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>4560</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>8800</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>6540</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>6000</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>8875</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>7950</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>5500</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>7475</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>7000</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>4880</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>5960</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>6840</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>7000</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>7482</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>9000</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>6000</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Linear_Regression!$E$6:$E$39</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="34"/>
-                <c:pt idx="0">
                   <c:v>13300000</c:v>
                 </c:pt>
                 <c:pt idx="1">
@@ -3182,10 +3070,10 @@
               </c:numCache>
             </c:numRef>
           </c:yVal>
-          <c:smooth val="1"/>
+          <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-1BEA-4014-9915-4EEED71A07B8}"/>
+              <c16:uniqueId val="{00000000-5F5E-4833-8F30-4D1BED234741}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3197,17 +3085,42 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="520453528"/>
-        <c:axId val="520454232"/>
+        <c:axId val="554109176"/>
+        <c:axId val="554115160"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="520453528"/>
+        <c:axId val="554109176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-IN"/>
+                  <a:t>Area</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3274,12 +3187,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="520454232"/>
+        <c:crossAx val="554115160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="520454232"/>
+        <c:axId val="554115160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3314,6 +3227,31 @@
           </c:spPr>
         </c:minorGridlines>
         <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-IN"/>
+                  <a:t>Price</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3380,7 +3318,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="520453528"/>
+        <c:crossAx val="554109176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3502,7 +3440,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-IN"/>
-              <a:t>error chart</a:t>
+              <a:t>Error</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -3569,125 +3507,113 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:xVal>
+          <c:yVal>
             <c:numRef>
-              <c:f>Linear_Regression!$B$6:$B$39</c:f>
+              <c:f>Linear_Regression!$F$6:$F$39</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="34"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>3985642.4948749878</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>2546642.2073515989</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>2880434.6877309158</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>2095642.4948749878</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5</c:v>
+                  <c:v>1515434.6877309158</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6</c:v>
+                  <c:v>542629.29128594138</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7</c:v>
+                  <c:v>383876.13415037468</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8</c:v>
+                  <c:v>907480.46900749393</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9</c:v>
+                  <c:v>725331.07168226875</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10</c:v>
+                  <c:v>215402.397566773</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>11</c:v>
+                  <c:v>-170344.58905935474</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>12</c:v>
+                  <c:v>-7227.48189827241</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>13</c:v>
+                  <c:v>-627162.90156998672</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>14</c:v>
+                  <c:v>287967.69670353085</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>15</c:v>
+                  <c:v>-206759.91582411155</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>16</c:v>
+                  <c:v>218695.02170778252</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>17</c:v>
+                  <c:v>-567419.14396027289</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>18</c:v>
+                  <c:v>-828493.98638457991</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>19</c:v>
+                  <c:v>53071.600275566801</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>20</c:v>
+                  <c:v>-1087942.1783602573</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>21</c:v>
+                  <c:v>-552071.62654021941</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>22</c:v>
+                  <c:v>-492668.92831773125</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>23</c:v>
+                  <c:v>-1281886.9975578245</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>24</c:v>
+                  <c:v>-1048234.227454491</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>25</c:v>
+                  <c:v>-429370.1336672809</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>26</c:v>
+                  <c:v>-928250.37253656238</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>27</c:v>
+                  <c:v>-808266.51761863381</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>28</c:v>
+                  <c:v>-377759.62830072269</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>29</c:v>
+                  <c:v>-755565.02474569529</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>30</c:v>
+                  <c:v>-1047850.90333049</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>31</c:v>
+                  <c:v>-1127326.5176186338</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>32</c:v>
+                  <c:v>-1287018.555661669</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>33</c:v>
+                  <c:v>-1733461.6962204371</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>34</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Linear_Regression!$I$6</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>3985642.4948749878</c:v>
+                  <c:v>-993168.92831773125</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3695,263 +3621,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-DF6D-4BB3-BD5A-6B9E97AB709B}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Linear_Regression!$B$6:$B$39</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="34"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>13</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>18</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>19</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>22</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>23</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>25</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>27</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>29</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>31</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>33</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>34</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Linear_Regression!$I$6:$I$39</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="34"/>
-                <c:pt idx="0">
-                  <c:v>3985642.4948749878</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2546642.2073515989</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2880434.6877309158</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2095642.4948749878</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1515434.6877309158</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>542629.29128594138</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>383876.13415037468</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>907480.46900749393</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>725331.07168226875</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>215402.397566773</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>-170344.58905935474</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>-7227.48189827241</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>-627162.90156998672</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>287967.69670353085</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>-206759.91582411155</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>218695.02170778252</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>-567419.14396027289</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>-828493.98638457991</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>53071.600275566801</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>-1087942.1783602573</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>-552071.62654021941</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>-492668.92831773125</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>-1281886.9975578245</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>-1048234.227454491</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>-429370.1336672809</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>-928250.37253656238</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>-808266.51761863381</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>-377759.62830072269</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>-755565.02474569529</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>-1047850.90333049</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>-1127326.5176186338</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>-1287018.555661669</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>-1733461.6962204371</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>-993168.92831773125</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-DF6D-4BB3-BD5A-6B9E97AB709B}"/>
+              <c16:uniqueId val="{00000000-4739-407F-A02E-DB2F2FF2B706}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3963,11 +3633,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="520505496"/>
-        <c:axId val="520503384"/>
+        <c:axId val="554107064"/>
+        <c:axId val="554109176"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="520505496"/>
+        <c:axId val="554107064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3987,7 +3657,6 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -4024,12 +3693,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="520503384"/>
+        <c:crossAx val="554109176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="520503384"/>
+        <c:axId val="554109176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4086,9 +3755,542 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="520505496"/>
+        <c:crossAx val="554107064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-IN"/>
+              <a:t>Price Vs Predicted(Price)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Linear_Regression!$D$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>price</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Linear_Regression!$D$6:$D$39</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="34"/>
+                <c:pt idx="0">
+                  <c:v>13300000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12250000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>12215000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11410000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10850000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10150000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9870000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9800000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9681000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9310000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9240000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9100000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>8960000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8890000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>8855000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8750000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8680000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>8645000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>8645000</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>8575000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>8540000</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>8463000</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>8400000</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>8400000</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>8400000</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>8400000</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>8400000</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>8295000</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>8190000</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>8120000</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>8080940</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>8043000</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>7980000</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>7962500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E602-44BC-BAA2-9A2F475590A9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Linear_Regression!$E$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Predicted(y)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Linear_Regression!$E$6:$E$39</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="34"/>
+                <c:pt idx="0">
+                  <c:v>9314357.5051250122</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9703357.7926484011</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9334565.3122690842</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9314357.5051250122</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9334565.3122690842</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9607370.7087140586</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9486123.8658496253</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8892519.5309925061</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8955668.9283177312</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9094597.602433227</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9410344.5890593547</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9107227.4818982724</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>9587162.9015699867</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8602032.3032964692</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>9061759.9158241116</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8531304.9782922175</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>9247419.1439602729</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>9473493.9863845799</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>8591928.3997244332</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>9662942.1783602573</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>9092071.6265402194</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>8955668.9283177312</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>9681886.9975578245</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>9448234.227454491</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>8829370.1336672809</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>9328250.3725365624</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>9208266.5176186338</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>8672759.6283007227</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>8945565.0247456953</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>9167850.90333049</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>9208266.5176186338</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>9330018.555661669</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>9713461.6962204371</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>8955668.9283177312</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-E602-44BC-BAA2-9A2F475590A9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="593910712"/>
+        <c:axId val="593913528"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="593910712"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="593913528"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="593913528"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="593910712"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -4413,6 +4615,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -7490,6 +7732,522 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -8457,23 +9215,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>18</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>312420</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>259080</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="10" name="Picture 9">
+        <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD5BA107-206F-E649-6F15-33FAE6AEB1F1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B59F0739-46D6-46AD-9F7D-48F51E2E7F54}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8506,8 +9264,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="10812780" y="922020"/>
-          <a:ext cx="2141220" cy="701040"/>
+          <a:off x="3482340" y="548640"/>
+          <a:ext cx="1082040" cy="205740"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8528,23 +9286,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>259080</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>815340</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>205740</xdr:rowOff>
+      <xdr:rowOff>22860</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="15" name="Picture 14">
+        <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{70422349-1213-4595-86FB-9E59C37578BC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D387F713-68AC-43D0-B533-4402C6BE9327}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8577,8 +9335,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="4945380" y="548640"/>
-          <a:ext cx="868680" cy="205740"/>
+          <a:off x="4305300" y="365760"/>
+          <a:ext cx="1455420" cy="205740"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8605,17 +9363,17 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>586740</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>22860</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>518160</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="17" name="Picture 16">
+        <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{88754CD5-6E1E-DB87-C7B6-E9FE529C2872}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4B2EEBBC-9A8F-4863-A00A-F1BFAAAD4D7A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8648,8 +9406,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="5768340" y="365760"/>
-          <a:ext cx="1196340" cy="205740"/>
+          <a:off x="6149340" y="365760"/>
+          <a:ext cx="1996440" cy="441960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8670,23 +9428,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>30480</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>68580</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>175260</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="19" name="Chart 18">
+        <xdr:cNvPr id="5" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9D4B81EA-22C5-538D-EA21-6123CA984097}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0690D131-E00E-8CD1-F73D-BBDE80C9D1FB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8706,23 +9464,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>441960</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>60960</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>144780</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="21" name="Chart 20">
+        <xdr:cNvPr id="6" name="Chart 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{71FF836A-A6E8-8365-2A30-D25F6FBF437A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{66202747-055B-15AB-4ED1-843C25B1CC5B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8735,6 +9493,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>472440</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>441960</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{07BCAF96-475B-B83B-050C-B31F8D50F3E5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -10982,7 +11776,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:J43"/>
   <sheetViews>
-    <sheetView topLeftCell="B16" workbookViewId="0">
+    <sheetView topLeftCell="B19" workbookViewId="0">
       <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
@@ -12374,18 +13168,18 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95E4E5C9-30C2-46DA-ADDA-91E751A0E456}">
-  <dimension ref="B4:P42"/>
+  <dimension ref="A3:P44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C4" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5:I5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.77734375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
     <col min="6" max="6" width="9.33203125" customWidth="1"/>
     <col min="7" max="8" width="12" bestFit="1" customWidth="1"/>
@@ -12395,1245 +13189,912 @@
     <col min="16" max="16" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:16" ht="17.399999999999999" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="C4" s="2" t="s">
+    <row r="3" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B3" s="52"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="52"/>
+      <c r="H3" s="52"/>
+    </row>
+    <row r="4" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="54"/>
+      <c r="C4" s="54" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="52"/>
+      <c r="F4" s="52"/>
+      <c r="G4" s="52"/>
+      <c r="H4" s="52"/>
+      <c r="L4" s="50" t="s">
+        <v>21</v>
+      </c>
+      <c r="M4" s="1">
+        <f>SUM(G6:G39)</f>
+        <v>55703400334254.453</v>
+      </c>
+    </row>
+    <row r="5" spans="2:16" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="B5" s="44" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" s="54"/>
+      <c r="I5" s="1"/>
+      <c r="L5" s="51"/>
+      <c r="M5" s="51"/>
+      <c r="N5" s="52"/>
+      <c r="O5" s="52"/>
+      <c r="P5" s="52"/>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B6" s="24">
+        <v>1</v>
+      </c>
+      <c r="C6" s="52">
+        <v>7420</v>
+      </c>
+      <c r="D6" s="52">
+        <v>13300000</v>
+      </c>
+      <c r="E6" s="52">
+        <v>9314357.5051250122</v>
+      </c>
+      <c r="F6" s="52">
+        <v>3985642.4948749878</v>
+      </c>
+      <c r="G6" s="25">
+        <v>15885346096953.316</v>
+      </c>
+      <c r="H6" s="52"/>
+      <c r="L6" s="52"/>
+      <c r="M6" s="52"/>
+      <c r="N6" s="52"/>
+      <c r="O6" s="53"/>
+      <c r="P6" s="52"/>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B7" s="24">
+        <v>2</v>
+      </c>
+      <c r="C7" s="52">
+        <v>8960</v>
+      </c>
+      <c r="D7" s="52">
+        <v>12250000</v>
+      </c>
+      <c r="E7" s="52">
+        <v>9703357.7926484011</v>
+      </c>
+      <c r="F7" s="52">
+        <v>2546642.2073515989</v>
+      </c>
+      <c r="G7" s="25">
+        <v>6485386532264.624</v>
+      </c>
+      <c r="H7" s="52"/>
+      <c r="L7" s="52"/>
+      <c r="M7" s="52"/>
+      <c r="N7" s="52"/>
+      <c r="O7" s="53"/>
+      <c r="P7" s="52"/>
+    </row>
+    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B8" s="24">
         <v>3</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="C8" s="52">
+        <v>7500</v>
+      </c>
+      <c r="D8" s="52">
+        <v>12215000</v>
+      </c>
+      <c r="E8" s="52">
+        <v>9334565.3122690842</v>
+      </c>
+      <c r="F8" s="52">
+        <v>2880434.6877309158</v>
+      </c>
+      <c r="G8" s="25">
+        <v>8296903990283.499</v>
+      </c>
+      <c r="H8" s="52"/>
+      <c r="L8" s="52"/>
+      <c r="M8" s="52"/>
+      <c r="N8" s="52"/>
+      <c r="O8" s="52"/>
+      <c r="P8" s="52"/>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B9" s="24">
+        <v>4</v>
+      </c>
+      <c r="C9" s="52">
+        <v>7420</v>
+      </c>
+      <c r="D9" s="52">
+        <v>11410000</v>
+      </c>
+      <c r="E9" s="52">
+        <v>9314357.5051250122</v>
+      </c>
+      <c r="F9" s="52">
+        <v>2095642.4948749878</v>
+      </c>
+      <c r="G9" s="25">
+        <v>4391717466325.8633</v>
+      </c>
+      <c r="H9" s="52"/>
+      <c r="L9" s="52"/>
+      <c r="M9" s="52"/>
+      <c r="N9" s="52"/>
+      <c r="O9" s="52"/>
+      <c r="P9" s="52"/>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B10" s="24">
+        <v>5</v>
+      </c>
+      <c r="C10" s="52">
+        <v>7500</v>
+      </c>
+      <c r="D10" s="52">
+        <v>10850000</v>
+      </c>
+      <c r="E10" s="52">
+        <v>9334565.3122690842</v>
+      </c>
+      <c r="F10" s="52">
+        <v>1515434.6877309158</v>
+      </c>
+      <c r="G10" s="25">
+        <v>2296542292778.0986</v>
+      </c>
+      <c r="H10" s="52"/>
+      <c r="L10" s="52"/>
+      <c r="M10" s="52"/>
+      <c r="N10" s="52"/>
+      <c r="O10" s="52"/>
+      <c r="P10" s="52"/>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B11" s="24">
+        <v>6</v>
+      </c>
+      <c r="C11" s="52">
+        <v>8580</v>
+      </c>
+      <c r="D11" s="52">
+        <v>10150000</v>
+      </c>
+      <c r="E11" s="52">
+        <v>9607370.7087140586</v>
+      </c>
+      <c r="F11" s="52">
+        <v>542629.29128594138</v>
+      </c>
+      <c r="G11" s="25">
+        <v>294446547761.48303</v>
+      </c>
+      <c r="H11" s="52"/>
+      <c r="L11" s="52"/>
+      <c r="M11" s="52"/>
+      <c r="N11" s="52"/>
+      <c r="O11" s="52"/>
+      <c r="P11" s="52"/>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B12" s="24">
+        <v>7</v>
+      </c>
+      <c r="C12" s="52">
+        <v>8100</v>
+      </c>
+      <c r="D12" s="52">
+        <v>9870000</v>
+      </c>
+      <c r="E12" s="52">
+        <v>9486123.8658496253</v>
+      </c>
+      <c r="F12" s="52">
+        <v>383876.13415037468</v>
+      </c>
+      <c r="G12" s="25">
+        <v>147360886370.23645</v>
+      </c>
+      <c r="H12" s="52"/>
+      <c r="L12" s="52"/>
+      <c r="M12" s="52"/>
+      <c r="N12" s="52"/>
+      <c r="O12" s="52"/>
+      <c r="P12" s="52"/>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B13" s="24">
+        <v>8</v>
+      </c>
+      <c r="C13" s="52">
+        <v>5750</v>
+      </c>
+      <c r="D13" s="52">
+        <v>9800000</v>
+      </c>
+      <c r="E13" s="52">
+        <v>8892519.5309925061</v>
+      </c>
+      <c r="F13" s="52">
+        <v>907480.46900749393</v>
+      </c>
+      <c r="G13" s="25">
+        <v>823520801630.06116</v>
+      </c>
+      <c r="H13" s="52"/>
+      <c r="L13" s="52"/>
+      <c r="M13" s="52"/>
+      <c r="N13" s="52"/>
+      <c r="O13" s="52"/>
+      <c r="P13" s="52"/>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B14" s="24">
+        <v>9</v>
+      </c>
+      <c r="C14" s="52">
+        <v>6000</v>
+      </c>
+      <c r="D14" s="52">
+        <v>9681000</v>
+      </c>
+      <c r="E14" s="52">
+        <v>8955668.9283177312</v>
+      </c>
+      <c r="F14" s="52">
+        <v>725331.07168226875</v>
+      </c>
+      <c r="G14" s="25">
+        <v>526105163547.74847</v>
+      </c>
+      <c r="H14" s="52"/>
+      <c r="L14" s="52"/>
+      <c r="M14" s="52"/>
+      <c r="N14" s="52"/>
+      <c r="O14" s="52"/>
+      <c r="P14" s="52"/>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B15" s="24">
+        <v>10</v>
+      </c>
+      <c r="C15" s="52">
+        <v>6550</v>
+      </c>
+      <c r="D15" s="52">
+        <v>9310000</v>
+      </c>
+      <c r="E15" s="52">
+        <v>9094597.602433227</v>
+      </c>
+      <c r="F15" s="52">
+        <v>215402.397566773</v>
+      </c>
+      <c r="G15" s="25">
+        <v>46398192877.514137</v>
+      </c>
+      <c r="H15" s="52"/>
+      <c r="L15" s="52"/>
+      <c r="M15" s="52"/>
+      <c r="N15" s="52"/>
+      <c r="O15" s="52"/>
+      <c r="P15" s="52"/>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="B16" s="24">
+        <v>11</v>
+      </c>
+      <c r="C16" s="52">
+        <v>7800</v>
+      </c>
+      <c r="D16" s="52">
+        <v>9240000</v>
+      </c>
+      <c r="E16" s="52">
+        <v>9410344.5890593547</v>
+      </c>
+      <c r="F16" s="52">
+        <v>-170344.58905935474</v>
+      </c>
+      <c r="G16" s="25">
+        <v>29017279021.800438</v>
+      </c>
+      <c r="H16" s="52"/>
+      <c r="L16" s="52"/>
+      <c r="M16" s="52"/>
+      <c r="N16" s="52"/>
+      <c r="O16" s="52"/>
+      <c r="P16" s="52"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B17" s="24">
+        <v>12</v>
+      </c>
+      <c r="C17" s="52">
+        <v>6600</v>
+      </c>
+      <c r="D17" s="52">
+        <v>9100000</v>
+      </c>
+      <c r="E17" s="52">
+        <v>9107227.4818982724</v>
+      </c>
+      <c r="F17" s="52">
+        <v>-7227.48189827241</v>
+      </c>
+      <c r="G17" s="25">
+        <v>52236494.589855358</v>
+      </c>
+      <c r="H17" s="52"/>
+      <c r="L17" s="52"/>
+      <c r="M17" s="52"/>
+      <c r="N17" s="52"/>
+      <c r="O17" s="52"/>
+      <c r="P17" s="52"/>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A18" s="52"/>
+      <c r="B18" s="24">
+        <v>13</v>
+      </c>
+      <c r="C18" s="52">
+        <v>8500</v>
+      </c>
+      <c r="D18" s="52">
+        <v>8960000</v>
+      </c>
+      <c r="E18" s="52">
+        <v>9587162.9015699867</v>
+      </c>
+      <c r="F18" s="52">
+        <v>-627162.90156998672</v>
+      </c>
+      <c r="G18" s="25">
+        <v>393333305105.68488</v>
+      </c>
+      <c r="H18" s="52"/>
+      <c r="L18" s="52"/>
+      <c r="M18" s="52"/>
+      <c r="N18" s="52"/>
+      <c r="O18" s="52"/>
+      <c r="P18" s="52"/>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A19" s="52"/>
+      <c r="B19" s="24">
+        <v>14</v>
+      </c>
+      <c r="C19" s="52">
+        <v>4600</v>
+      </c>
+      <c r="D19" s="52">
+        <v>8890000</v>
+      </c>
+      <c r="E19" s="52">
+        <v>8602032.3032964692</v>
+      </c>
+      <c r="F19" s="52">
+        <v>287967.69670353085</v>
+      </c>
+      <c r="G19" s="25">
+        <v>82925394344.736725</v>
+      </c>
+      <c r="H19" s="52"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A20" s="52"/>
+      <c r="B20" s="24">
+        <v>15</v>
+      </c>
+      <c r="C20" s="52">
+        <v>6420</v>
+      </c>
+      <c r="D20" s="52">
+        <v>8855000</v>
+      </c>
+      <c r="E20" s="52">
+        <v>9061759.9158241116</v>
+      </c>
+      <c r="F20" s="52">
+        <v>-206759.91582411155</v>
+      </c>
+      <c r="G20" s="25">
+        <v>42749662791.593697</v>
+      </c>
+      <c r="H20" s="52"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A21" s="52"/>
+      <c r="B21" s="24">
+        <v>16</v>
+      </c>
+      <c r="C21" s="52">
+        <v>4320</v>
+      </c>
+      <c r="D21" s="52">
+        <v>8750000</v>
+      </c>
+      <c r="E21" s="52">
+        <v>8531304.9782922175</v>
+      </c>
+      <c r="F21" s="52">
+        <v>218695.02170778252</v>
+      </c>
+      <c r="G21" s="25">
+        <v>47827512519.767471</v>
+      </c>
+      <c r="H21" s="52"/>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A22" s="52"/>
+      <c r="B22" s="24">
+        <v>17</v>
+      </c>
+      <c r="C22" s="52">
+        <v>7155</v>
+      </c>
+      <c r="D22" s="52">
+        <v>8680000</v>
+      </c>
+      <c r="E22" s="52">
+        <v>9247419.1439602729</v>
+      </c>
+      <c r="F22" s="52">
+        <v>-567419.14396027289</v>
+      </c>
+      <c r="G22" s="25">
+        <v>321964484932.60889</v>
+      </c>
+      <c r="H22" s="52"/>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A23" s="52"/>
+      <c r="B23" s="24">
+        <v>18</v>
+      </c>
+      <c r="C23" s="52">
+        <v>8050</v>
+      </c>
+      <c r="D23" s="52">
+        <v>8645000</v>
+      </c>
+      <c r="E23" s="52">
+        <v>9473493.9863845799</v>
+      </c>
+      <c r="F23" s="52">
+        <v>-828493.98638457991</v>
+      </c>
+      <c r="G23" s="25">
+        <v>686402285475.41248</v>
+      </c>
+      <c r="H23" s="52"/>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A24" s="52"/>
+      <c r="B24" s="24">
+        <v>19</v>
+      </c>
+      <c r="C24" s="52">
+        <v>4560</v>
+      </c>
+      <c r="D24" s="52">
+        <v>8645000</v>
+      </c>
+      <c r="E24" s="52">
+        <v>8591928.3997244332</v>
+      </c>
+      <c r="F24" s="52">
+        <v>53071.600275566801</v>
+      </c>
+      <c r="G24" s="25">
+        <v>2816594755.8095422</v>
+      </c>
+      <c r="H24" s="52"/>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A25" s="52"/>
+      <c r="B25" s="24">
+        <v>20</v>
+      </c>
+      <c r="C25" s="52">
+        <v>8800</v>
+      </c>
+      <c r="D25" s="52">
+        <v>8575000</v>
+      </c>
+      <c r="E25" s="52">
+        <v>9662942.1783602573</v>
+      </c>
+      <c r="F25" s="52">
+        <v>-1087942.1783602573</v>
+      </c>
+      <c r="G25" s="25">
+        <v>1183618183455.262</v>
+      </c>
+      <c r="H25" s="52"/>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A26" s="52"/>
+      <c r="B26" s="24">
         <v>21</v>
       </c>
-      <c r="G4" t="s">
+      <c r="C26" s="52">
+        <v>6540</v>
+      </c>
+      <c r="D26" s="52">
+        <v>8540000</v>
+      </c>
+      <c r="E26" s="52">
+        <v>9092071.6265402194</v>
+      </c>
+      <c r="F26" s="52">
+        <v>-552071.62654021941</v>
+      </c>
+      <c r="G26" s="25">
+        <v>304783080830.76349</v>
+      </c>
+      <c r="H26" s="52"/>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A27" s="52"/>
+      <c r="B27" s="24">
+        <v>22</v>
+      </c>
+      <c r="C27" s="52">
+        <v>6000</v>
+      </c>
+      <c r="D27" s="52">
+        <v>8463000</v>
+      </c>
+      <c r="E27" s="52">
+        <v>8955668.9283177312</v>
+      </c>
+      <c r="F27" s="52">
+        <v>-492668.92831773125</v>
+      </c>
+      <c r="G27" s="25">
+        <v>242722672929.74182</v>
+      </c>
+      <c r="H27" s="52"/>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A28" s="52"/>
+      <c r="B28" s="24">
         <v>23</v>
       </c>
-    </row>
-    <row r="5" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="D5" s="31" t="s">
-        <v>1</v>
-      </c>
-      <c r="E5" s="30"/>
-      <c r="F5" s="50"/>
-      <c r="G5" s="51"/>
-      <c r="H5" s="1" t="s">
+      <c r="C28" s="52">
+        <v>8875</v>
+      </c>
+      <c r="D28" s="52">
+        <v>8400000</v>
+      </c>
+      <c r="E28" s="52">
+        <v>9681886.9975578245</v>
+      </c>
+      <c r="F28" s="52">
+        <v>-1281886.9975578245</v>
+      </c>
+      <c r="G28" s="25">
+        <v>1643234274507.814</v>
+      </c>
+      <c r="H28" s="52"/>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A29" s="52"/>
+      <c r="B29" s="24">
+        <v>24</v>
+      </c>
+      <c r="C29" s="52">
+        <v>7950</v>
+      </c>
+      <c r="D29" s="52">
+        <v>8400000</v>
+      </c>
+      <c r="E29" s="52">
+        <v>9448234.227454491</v>
+      </c>
+      <c r="F29" s="52">
+        <v>-1048234.227454491</v>
+      </c>
+      <c r="G29" s="25">
+        <v>1098794995607.1135</v>
+      </c>
+      <c r="H29" s="52"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A30" s="52"/>
+      <c r="B30" s="24">
+        <v>25</v>
+      </c>
+      <c r="C30" s="52">
+        <v>5500</v>
+      </c>
+      <c r="D30" s="52">
+        <v>8400000</v>
+      </c>
+      <c r="E30" s="52">
+        <v>8829370.1336672809</v>
+      </c>
+      <c r="F30" s="52">
+        <v>-429370.1336672809</v>
+      </c>
+      <c r="G30" s="25">
+        <v>184358711685.45868</v>
+      </c>
+      <c r="H30" s="52"/>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A31" s="52"/>
+      <c r="B31" s="24">
+        <v>26</v>
+      </c>
+      <c r="C31" s="52">
+        <v>7475</v>
+      </c>
+      <c r="D31" s="52">
+        <v>8400000</v>
+      </c>
+      <c r="E31" s="52">
+        <v>9328250.3725365624</v>
+      </c>
+      <c r="F31" s="52">
+        <v>-928250.37253656238</v>
+      </c>
+      <c r="G31" s="25">
+        <v>861648754114.26685</v>
+      </c>
+      <c r="H31" s="52"/>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A32" s="52"/>
+      <c r="B32" s="24">
+        <v>27</v>
+      </c>
+      <c r="C32" s="52">
+        <v>7000</v>
+      </c>
+      <c r="D32" s="52">
+        <v>8400000</v>
+      </c>
+      <c r="E32" s="52">
+        <v>9208266.5176186338</v>
+      </c>
+      <c r="F32" s="52">
+        <v>-808266.51761863381</v>
+      </c>
+      <c r="G32" s="25">
+        <v>653294763503.35327</v>
+      </c>
+      <c r="H32" s="52"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A33" s="52"/>
+      <c r="B33" s="24">
+        <v>28</v>
+      </c>
+      <c r="C33" s="52">
+        <v>4880</v>
+      </c>
+      <c r="D33" s="52">
+        <v>8295000</v>
+      </c>
+      <c r="E33" s="52">
+        <v>8672759.6283007227</v>
+      </c>
+      <c r="F33" s="52">
+        <v>-377759.62830072269</v>
+      </c>
+      <c r="G33" s="25">
+        <v>142702336773.90018</v>
+      </c>
+      <c r="H33" s="52"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A34" s="52"/>
+      <c r="B34" s="24">
+        <v>29</v>
+      </c>
+      <c r="C34" s="52">
+        <v>5960</v>
+      </c>
+      <c r="D34" s="52">
+        <v>8190000</v>
+      </c>
+      <c r="E34" s="52">
+        <v>8945565.0247456953</v>
+      </c>
+      <c r="F34" s="52">
+        <v>-755565.02474569529</v>
+      </c>
+      <c r="G34" s="25">
+        <v>570878506618.96313</v>
+      </c>
+      <c r="H34" s="52"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A35" s="52"/>
+      <c r="B35" s="24">
+        <v>30</v>
+      </c>
+      <c r="C35" s="52">
+        <v>6840</v>
+      </c>
+      <c r="D35" s="52">
+        <v>8120000</v>
+      </c>
+      <c r="E35" s="52">
+        <v>9167850.90333049</v>
+      </c>
+      <c r="F35" s="52">
+        <v>-1047850.90333049</v>
+      </c>
+      <c r="G35" s="25">
+        <v>1097991515610.5239</v>
+      </c>
+      <c r="H35" s="52"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A36" s="52"/>
+      <c r="B36" s="24">
+        <v>31</v>
+      </c>
+      <c r="C36" s="52">
+        <v>7000</v>
+      </c>
+      <c r="D36" s="52">
+        <v>8080940</v>
+      </c>
+      <c r="E36" s="52">
+        <v>9208266.5176186338</v>
+      </c>
+      <c r="F36" s="52">
+        <v>-1127326.5176186338</v>
+      </c>
+      <c r="G36" s="25">
+        <v>1270865077326.1558</v>
+      </c>
+      <c r="H36" s="52"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A37" s="52"/>
+      <c r="B37" s="24">
         <v>32</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="C37" s="52">
+        <v>7482</v>
+      </c>
+      <c r="D37" s="52">
+        <v>8043000</v>
+      </c>
+      <c r="E37" s="52">
+        <v>9330018.555661669</v>
+      </c>
+      <c r="F37" s="52">
+        <v>-1287018.555661669</v>
+      </c>
+      <c r="G37" s="25">
+        <v>1656416762617.4485</v>
+      </c>
+      <c r="H37" s="52"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A38" s="52"/>
+      <c r="B38" s="24">
         <v>33</v>
       </c>
-      <c r="L5" s="59" t="s">
-        <v>24</v>
-      </c>
-      <c r="M5" s="59"/>
-      <c r="N5" t="s">
-        <v>3</v>
-      </c>
-      <c r="O5" t="s">
-        <v>25</v>
-      </c>
-      <c r="P5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="2:16" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="B6" s="34">
-        <v>1</v>
-      </c>
-      <c r="C6" s="35">
-        <v>13300000</v>
-      </c>
-      <c r="D6" s="36">
-        <v>7420</v>
-      </c>
-      <c r="E6" s="35">
-        <f>C6</f>
-        <v>13300000</v>
-      </c>
-      <c r="F6">
-        <f>D6*D6</f>
-        <v>55056400</v>
-      </c>
-      <c r="G6" s="25">
-        <f>C6*D6</f>
-        <v>98686000000</v>
-      </c>
-      <c r="H6">
-        <f>M$15+M$16*D6</f>
-        <v>9314357.5051250122</v>
-      </c>
-      <c r="I6">
-        <f>C6-H6</f>
-        <v>3985642.4948749878</v>
-      </c>
-      <c r="L6" s="53">
-        <f>B39</f>
+      <c r="C38" s="52">
+        <v>9000</v>
+      </c>
+      <c r="D38" s="52">
+        <v>7980000</v>
+      </c>
+      <c r="E38" s="52">
+        <v>9713461.6962204371</v>
+      </c>
+      <c r="F38" s="52">
+        <v>-1733461.6962204371</v>
+      </c>
+      <c r="G38" s="25">
+        <v>3004889452263.4351</v>
+      </c>
+      <c r="H38" s="52"/>
+    </row>
+    <row r="39" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="52"/>
+      <c r="B39" s="26">
         <v>34</v>
       </c>
-      <c r="M6" s="54">
-        <f>D40</f>
-        <v>237087</v>
-      </c>
-      <c r="N6" s="57" t="s">
-        <v>27</v>
-      </c>
-      <c r="O6" s="60" t="s">
-        <v>25</v>
-      </c>
-      <c r="P6" s="57">
-        <f>C40</f>
-        <v>312850440</v>
-      </c>
-    </row>
-    <row r="7" spans="2:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="34">
-        <f>B6+1</f>
-        <v>2</v>
-      </c>
-      <c r="C7" s="35">
-        <v>12250000</v>
-      </c>
-      <c r="D7" s="36">
-        <v>8960</v>
-      </c>
-      <c r="E7" s="35">
-        <f t="shared" ref="E7:E39" si="0">C7</f>
-        <v>12250000</v>
-      </c>
-      <c r="F7">
-        <f t="shared" ref="F7:F39" si="1">D7*D7</f>
-        <v>80281600</v>
-      </c>
-      <c r="G7" s="25">
-        <f t="shared" ref="G7:G39" si="2">C7*D7</f>
-        <v>109760000000</v>
-      </c>
-      <c r="H7">
-        <f t="shared" ref="H7:H39" si="3">M$15+M$16*D7</f>
-        <v>9703357.7926484011</v>
-      </c>
-      <c r="I7">
-        <f t="shared" ref="I7:I39" si="4">C7-H7</f>
-        <v>2546642.2073515989</v>
-      </c>
-      <c r="L7" s="55">
-        <f>D40</f>
-        <v>237087</v>
-      </c>
-      <c r="M7" s="56">
-        <f>F40</f>
-        <v>1709971999</v>
-      </c>
-      <c r="N7" s="58" t="s">
-        <v>28</v>
-      </c>
-      <c r="O7" s="60"/>
-      <c r="P7" s="58">
-        <f>G40</f>
-        <v>2195881856000</v>
-      </c>
-    </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B8" s="34">
-        <f t="shared" ref="B8:B39" si="5">B7+1</f>
-        <v>3</v>
-      </c>
-      <c r="C8" s="35">
-        <v>12215000</v>
-      </c>
-      <c r="D8" s="36">
-        <v>7500</v>
-      </c>
-      <c r="E8" s="35">
-        <f t="shared" si="0"/>
-        <v>12215000</v>
-      </c>
-      <c r="F8">
-        <f t="shared" si="1"/>
-        <v>56250000</v>
-      </c>
-      <c r="G8" s="25">
-        <f t="shared" si="2"/>
-        <v>91612500000</v>
-      </c>
-      <c r="H8">
-        <f t="shared" si="3"/>
-        <v>9334565.3122690842</v>
-      </c>
-      <c r="I8">
-        <f t="shared" si="4"/>
-        <v>2880434.6877309158</v>
-      </c>
-    </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B9" s="34">
-        <f t="shared" si="5"/>
-        <v>4</v>
-      </c>
-      <c r="C9" s="35">
-        <v>11410000</v>
-      </c>
-      <c r="D9" s="36">
-        <v>7420</v>
-      </c>
-      <c r="E9" s="35">
-        <f t="shared" si="0"/>
-        <v>11410000</v>
-      </c>
-      <c r="F9">
-        <f t="shared" si="1"/>
-        <v>55056400</v>
-      </c>
-      <c r="G9" s="25">
-        <f t="shared" si="2"/>
-        <v>84662200000</v>
-      </c>
-      <c r="H9">
-        <f t="shared" si="3"/>
-        <v>9314357.5051250122</v>
-      </c>
-      <c r="I9">
-        <f t="shared" si="4"/>
-        <v>2095642.4948749878</v>
-      </c>
-    </row>
-    <row r="10" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="34">
-        <f t="shared" si="5"/>
-        <v>5</v>
-      </c>
-      <c r="C10" s="35">
-        <v>10850000</v>
-      </c>
-      <c r="D10" s="36">
-        <v>7500</v>
-      </c>
-      <c r="E10" s="35">
-        <f t="shared" si="0"/>
-        <v>10850000</v>
-      </c>
-      <c r="F10">
-        <f t="shared" si="1"/>
-        <v>56250000</v>
-      </c>
-      <c r="G10" s="25">
-        <f t="shared" si="2"/>
-        <v>81375000000</v>
-      </c>
-      <c r="H10">
-        <f t="shared" si="3"/>
-        <v>9334565.3122690842</v>
-      </c>
-      <c r="I10">
-        <f t="shared" si="4"/>
-        <v>1515434.6877309158</v>
-      </c>
-      <c r="L10" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="34">
-        <f t="shared" si="5"/>
-        <v>6</v>
-      </c>
-      <c r="C11" s="35">
-        <v>10150000</v>
-      </c>
-      <c r="D11" s="36">
-        <v>8580</v>
-      </c>
-      <c r="E11" s="35">
-        <f t="shared" si="0"/>
-        <v>10150000</v>
-      </c>
-      <c r="F11">
-        <f t="shared" si="1"/>
-        <v>73616400</v>
-      </c>
-      <c r="G11" s="25">
-        <f t="shared" si="2"/>
-        <v>87087000000</v>
-      </c>
-      <c r="H11">
-        <f t="shared" si="3"/>
-        <v>9607370.7087140586</v>
-      </c>
-      <c r="I11">
-        <f t="shared" si="4"/>
-        <v>542629.29128594138</v>
-      </c>
-      <c r="L11" s="52">
-        <f t="array" ref="L11:M12">MINVERSE(L6:M7)</f>
-        <v>0.886545973636095</v>
-      </c>
-      <c r="M11" s="52">
-        <v>-1.2291927901414765E-4</v>
-      </c>
-    </row>
-    <row r="12" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="34">
-        <f t="shared" si="5"/>
-        <v>7</v>
-      </c>
-      <c r="C12" s="35">
-        <v>9870000</v>
-      </c>
-      <c r="D12" s="36">
-        <v>8100</v>
-      </c>
-      <c r="E12" s="35">
-        <f t="shared" si="0"/>
-        <v>9870000</v>
-      </c>
-      <c r="F12">
-        <f t="shared" si="1"/>
-        <v>65610000</v>
-      </c>
-      <c r="G12" s="25">
-        <f t="shared" si="2"/>
-        <v>79947000000</v>
-      </c>
-      <c r="H12">
-        <f t="shared" si="3"/>
-        <v>9486123.8658496253</v>
-      </c>
-      <c r="I12">
-        <f t="shared" si="4"/>
-        <v>383876.13415037468</v>
-      </c>
-      <c r="L12" s="52">
-        <v>-1.2291927901414768E-4</v>
-      </c>
-      <c r="M12" s="52">
-        <v>1.7627518533200979E-8</v>
-      </c>
-    </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B13" s="34">
-        <f t="shared" si="5"/>
-        <v>8</v>
-      </c>
-      <c r="C13" s="35">
-        <v>9800000</v>
-      </c>
-      <c r="D13" s="36">
-        <v>5750</v>
-      </c>
-      <c r="E13" s="35">
-        <f t="shared" si="0"/>
-        <v>9800000</v>
-      </c>
-      <c r="F13">
-        <f t="shared" si="1"/>
-        <v>33062500</v>
-      </c>
-      <c r="G13" s="25">
-        <f t="shared" si="2"/>
-        <v>56350000000</v>
-      </c>
-      <c r="H13">
-        <f t="shared" si="3"/>
-        <v>8892519.5309925061</v>
-      </c>
-      <c r="I13">
-        <f t="shared" si="4"/>
-        <v>907480.46900749393</v>
-      </c>
-    </row>
-    <row r="14" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="34">
-        <f t="shared" si="5"/>
-        <v>9</v>
-      </c>
-      <c r="C14" s="35">
-        <v>9681000</v>
-      </c>
-      <c r="D14" s="36">
+      <c r="C39" s="27">
         <v>6000</v>
       </c>
-      <c r="E14" s="35">
-        <f t="shared" si="0"/>
-        <v>9681000</v>
-      </c>
-      <c r="F14">
-        <f t="shared" si="1"/>
-        <v>36000000</v>
-      </c>
-      <c r="G14" s="25">
-        <f t="shared" si="2"/>
-        <v>58086000000</v>
-      </c>
-      <c r="H14">
-        <f t="shared" si="3"/>
+      <c r="D39" s="27">
+        <v>7962500</v>
+      </c>
+      <c r="E39" s="27">
         <v>8955668.9283177312</v>
       </c>
-      <c r="I14">
-        <f t="shared" si="4"/>
-        <v>725331.07168226875</v>
-      </c>
-      <c r="L14" t="s">
-        <v>31</v>
-      </c>
-      <c r="M14" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" spans="2:16" ht="15.6" x14ac:dyDescent="0.35">
-      <c r="B15" s="34">
-        <f t="shared" si="5"/>
-        <v>10</v>
-      </c>
-      <c r="C15" s="35">
-        <v>9310000</v>
-      </c>
-      <c r="D15" s="36">
-        <v>6550</v>
-      </c>
-      <c r="E15" s="35">
-        <f t="shared" si="0"/>
-        <v>9310000</v>
-      </c>
-      <c r="F15">
-        <f t="shared" si="1"/>
-        <v>42902500</v>
-      </c>
-      <c r="G15" s="25">
-        <f t="shared" si="2"/>
-        <v>60980500000</v>
-      </c>
-      <c r="H15">
-        <f t="shared" si="3"/>
-        <v>9094597.602433227</v>
-      </c>
-      <c r="I15">
-        <f t="shared" si="4"/>
-        <v>215402.397566773</v>
-      </c>
-      <c r="L15" s="57" t="s">
-        <v>27</v>
-      </c>
-      <c r="M15">
-        <f t="array" ref="M15:M16">MMULT(L11:M12, P6:P7)</f>
-        <v>7440083.3925123215</v>
-      </c>
-    </row>
-    <row r="16" spans="2:16" ht="16.2" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B16" s="34">
-        <f t="shared" si="5"/>
-        <v>11</v>
-      </c>
-      <c r="C16" s="35">
-        <v>9240000</v>
-      </c>
-      <c r="D16" s="36">
-        <v>7800</v>
-      </c>
-      <c r="E16" s="35">
-        <f t="shared" si="0"/>
-        <v>9240000</v>
-      </c>
-      <c r="F16">
-        <f t="shared" si="1"/>
-        <v>60840000</v>
-      </c>
-      <c r="G16" s="25">
-        <f t="shared" si="2"/>
-        <v>72072000000</v>
-      </c>
-      <c r="H16">
-        <f t="shared" si="3"/>
-        <v>9410344.5890593547</v>
-      </c>
-      <c r="I16">
-        <f t="shared" si="4"/>
-        <v>-170344.58905935474</v>
-      </c>
-      <c r="L16" s="58" t="s">
-        <v>28</v>
-      </c>
-      <c r="M16">
-        <v>252.59758930090175</v>
-      </c>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B17" s="34">
-        <f t="shared" si="5"/>
-        <v>12</v>
-      </c>
-      <c r="C17" s="35">
-        <v>9100000</v>
-      </c>
-      <c r="D17" s="36">
-        <v>6600</v>
-      </c>
-      <c r="E17" s="35">
-        <f t="shared" si="0"/>
-        <v>9100000</v>
-      </c>
-      <c r="F17">
-        <f t="shared" si="1"/>
-        <v>43560000</v>
-      </c>
-      <c r="G17" s="25">
-        <f t="shared" si="2"/>
-        <v>60060000000</v>
-      </c>
-      <c r="H17">
-        <f t="shared" si="3"/>
-        <v>9107227.4818982724</v>
-      </c>
-      <c r="I17">
-        <f t="shared" si="4"/>
-        <v>-7227.48189827241</v>
-      </c>
-    </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B18" s="34">
-        <f t="shared" si="5"/>
-        <v>13</v>
-      </c>
-      <c r="C18" s="35">
-        <v>8960000</v>
-      </c>
-      <c r="D18" s="36">
-        <v>8500</v>
-      </c>
-      <c r="E18" s="35">
-        <f t="shared" si="0"/>
-        <v>8960000</v>
-      </c>
-      <c r="F18">
-        <f t="shared" si="1"/>
-        <v>72250000</v>
-      </c>
-      <c r="G18" s="25">
-        <f t="shared" si="2"/>
-        <v>76160000000</v>
-      </c>
-      <c r="H18">
-        <f t="shared" si="3"/>
-        <v>9587162.9015699867</v>
-      </c>
-      <c r="I18">
-        <f t="shared" si="4"/>
-        <v>-627162.90156998672</v>
-      </c>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B19" s="34">
-        <f t="shared" si="5"/>
-        <v>14</v>
-      </c>
-      <c r="C19" s="35">
-        <v>8890000</v>
-      </c>
-      <c r="D19" s="36">
-        <v>4600</v>
-      </c>
-      <c r="E19" s="35">
-        <f t="shared" si="0"/>
-        <v>8890000</v>
-      </c>
-      <c r="F19">
-        <f t="shared" si="1"/>
-        <v>21160000</v>
-      </c>
-      <c r="G19" s="25">
-        <f t="shared" si="2"/>
-        <v>40894000000</v>
-      </c>
-      <c r="H19">
-        <f t="shared" si="3"/>
-        <v>8602032.3032964692</v>
-      </c>
-      <c r="I19">
-        <f t="shared" si="4"/>
-        <v>287967.69670353085</v>
-      </c>
-    </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B20" s="34">
-        <f t="shared" si="5"/>
-        <v>15</v>
-      </c>
-      <c r="C20" s="35">
-        <v>8855000</v>
-      </c>
-      <c r="D20" s="36">
-        <v>6420</v>
-      </c>
-      <c r="E20" s="35">
-        <f t="shared" si="0"/>
-        <v>8855000</v>
-      </c>
-      <c r="F20">
-        <f t="shared" si="1"/>
-        <v>41216400</v>
-      </c>
-      <c r="G20" s="25">
-        <f t="shared" si="2"/>
-        <v>56849100000</v>
-      </c>
-      <c r="H20">
-        <f t="shared" si="3"/>
-        <v>9061759.9158241116</v>
-      </c>
-      <c r="I20">
-        <f t="shared" si="4"/>
-        <v>-206759.91582411155</v>
-      </c>
-    </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B21" s="34">
-        <f t="shared" si="5"/>
-        <v>16</v>
-      </c>
-      <c r="C21" s="35">
-        <v>8750000</v>
-      </c>
-      <c r="D21" s="36">
-        <v>4320</v>
-      </c>
-      <c r="E21" s="35">
-        <f t="shared" si="0"/>
-        <v>8750000</v>
-      </c>
-      <c r="F21">
-        <f t="shared" si="1"/>
-        <v>18662400</v>
-      </c>
-      <c r="G21" s="25">
-        <f t="shared" si="2"/>
-        <v>37800000000</v>
-      </c>
-      <c r="H21">
-        <f t="shared" si="3"/>
-        <v>8531304.9782922175</v>
-      </c>
-      <c r="I21">
-        <f t="shared" si="4"/>
-        <v>218695.02170778252</v>
-      </c>
-    </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B22" s="34">
-        <f t="shared" si="5"/>
-        <v>17</v>
-      </c>
-      <c r="C22" s="35">
-        <v>8680000</v>
-      </c>
-      <c r="D22" s="36">
-        <v>7155</v>
-      </c>
-      <c r="E22" s="35">
-        <f t="shared" si="0"/>
-        <v>8680000</v>
-      </c>
-      <c r="F22">
-        <f t="shared" si="1"/>
-        <v>51194025</v>
-      </c>
-      <c r="G22" s="25">
-        <f t="shared" si="2"/>
-        <v>62105400000</v>
-      </c>
-      <c r="H22">
-        <f t="shared" si="3"/>
-        <v>9247419.1439602729</v>
-      </c>
-      <c r="I22">
-        <f t="shared" si="4"/>
-        <v>-567419.14396027289</v>
-      </c>
-    </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B23" s="34">
-        <f t="shared" si="5"/>
-        <v>18</v>
-      </c>
-      <c r="C23" s="35">
-        <v>8645000</v>
-      </c>
-      <c r="D23" s="36">
-        <v>8050</v>
-      </c>
-      <c r="E23" s="35">
-        <f t="shared" si="0"/>
-        <v>8645000</v>
-      </c>
-      <c r="F23">
-        <f t="shared" si="1"/>
-        <v>64802500</v>
-      </c>
-      <c r="G23" s="25">
-        <f t="shared" si="2"/>
-        <v>69592250000</v>
-      </c>
-      <c r="H23">
-        <f t="shared" si="3"/>
-        <v>9473493.9863845799</v>
-      </c>
-      <c r="I23">
-        <f t="shared" si="4"/>
-        <v>-828493.98638457991</v>
-      </c>
-    </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B24" s="34">
-        <f t="shared" si="5"/>
-        <v>19</v>
-      </c>
-      <c r="C24" s="35">
-        <v>8645000</v>
-      </c>
-      <c r="D24" s="36">
-        <v>4560</v>
-      </c>
-      <c r="E24" s="35">
-        <f t="shared" si="0"/>
-        <v>8645000</v>
-      </c>
-      <c r="F24">
-        <f t="shared" si="1"/>
-        <v>20793600</v>
-      </c>
-      <c r="G24" s="25">
-        <f t="shared" si="2"/>
-        <v>39421200000</v>
-      </c>
-      <c r="H24">
-        <f t="shared" si="3"/>
-        <v>8591928.3997244332</v>
-      </c>
-      <c r="I24">
-        <f t="shared" si="4"/>
-        <v>53071.600275566801</v>
-      </c>
-    </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B25" s="34">
-        <f t="shared" si="5"/>
-        <v>20</v>
-      </c>
-      <c r="C25" s="35">
-        <v>8575000</v>
-      </c>
-      <c r="D25" s="36">
-        <v>8800</v>
-      </c>
-      <c r="E25" s="35">
-        <f t="shared" si="0"/>
-        <v>8575000</v>
-      </c>
-      <c r="F25">
-        <f t="shared" si="1"/>
-        <v>77440000</v>
-      </c>
-      <c r="G25" s="25">
-        <f t="shared" si="2"/>
-        <v>75460000000</v>
-      </c>
-      <c r="H25">
-        <f t="shared" si="3"/>
-        <v>9662942.1783602573</v>
-      </c>
-      <c r="I25">
-        <f t="shared" si="4"/>
-        <v>-1087942.1783602573</v>
-      </c>
-    </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B26" s="34">
-        <f t="shared" si="5"/>
-        <v>21</v>
-      </c>
-      <c r="C26" s="35">
-        <v>8540000</v>
-      </c>
-      <c r="D26" s="36">
-        <v>6540</v>
-      </c>
-      <c r="E26" s="35">
-        <f t="shared" si="0"/>
-        <v>8540000</v>
-      </c>
-      <c r="F26">
-        <f t="shared" si="1"/>
-        <v>42771600</v>
-      </c>
-      <c r="G26" s="25">
-        <f t="shared" si="2"/>
-        <v>55851600000</v>
-      </c>
-      <c r="H26">
-        <f t="shared" si="3"/>
-        <v>9092071.6265402194</v>
-      </c>
-      <c r="I26">
-        <f t="shared" si="4"/>
-        <v>-552071.62654021941</v>
-      </c>
-    </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B27" s="34">
-        <f t="shared" si="5"/>
-        <v>22</v>
-      </c>
-      <c r="C27" s="35">
-        <v>8463000</v>
-      </c>
-      <c r="D27" s="36">
-        <v>6000</v>
-      </c>
-      <c r="E27" s="35">
-        <f t="shared" si="0"/>
-        <v>8463000</v>
-      </c>
-      <c r="F27">
-        <f t="shared" si="1"/>
-        <v>36000000</v>
-      </c>
-      <c r="G27" s="25">
-        <f t="shared" si="2"/>
-        <v>50778000000</v>
-      </c>
-      <c r="H27">
-        <f t="shared" si="3"/>
-        <v>8955668.9283177312</v>
-      </c>
-      <c r="I27">
-        <f t="shared" si="4"/>
-        <v>-492668.92831773125</v>
-      </c>
-    </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B28" s="34">
-        <f t="shared" si="5"/>
-        <v>23</v>
-      </c>
-      <c r="C28" s="35">
-        <v>8400000</v>
-      </c>
-      <c r="D28" s="36">
-        <v>8875</v>
-      </c>
-      <c r="E28" s="35">
-        <f t="shared" si="0"/>
-        <v>8400000</v>
-      </c>
-      <c r="F28">
-        <f t="shared" si="1"/>
-        <v>78765625</v>
-      </c>
-      <c r="G28" s="25">
-        <f t="shared" si="2"/>
-        <v>74550000000</v>
-      </c>
-      <c r="H28">
-        <f t="shared" si="3"/>
-        <v>9681886.9975578245</v>
-      </c>
-      <c r="I28">
-        <f t="shared" si="4"/>
-        <v>-1281886.9975578245</v>
-      </c>
-    </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B29" s="34">
-        <f t="shared" si="5"/>
-        <v>24</v>
-      </c>
-      <c r="C29" s="35">
-        <v>8400000</v>
-      </c>
-      <c r="D29" s="36">
-        <v>7950</v>
-      </c>
-      <c r="E29" s="35">
-        <f t="shared" si="0"/>
-        <v>8400000</v>
-      </c>
-      <c r="F29">
-        <f t="shared" si="1"/>
-        <v>63202500</v>
-      </c>
-      <c r="G29" s="25">
-        <f t="shared" si="2"/>
-        <v>66780000000</v>
-      </c>
-      <c r="H29">
-        <f t="shared" si="3"/>
-        <v>9448234.227454491</v>
-      </c>
-      <c r="I29">
-        <f t="shared" si="4"/>
-        <v>-1048234.227454491</v>
-      </c>
-    </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B30" s="34">
-        <f t="shared" si="5"/>
-        <v>25</v>
-      </c>
-      <c r="C30" s="35">
-        <v>8400000</v>
-      </c>
-      <c r="D30" s="36">
-        <v>5500</v>
-      </c>
-      <c r="E30" s="35">
-        <f t="shared" si="0"/>
-        <v>8400000</v>
-      </c>
-      <c r="F30">
-        <f t="shared" si="1"/>
-        <v>30250000</v>
-      </c>
-      <c r="G30" s="25">
-        <f t="shared" si="2"/>
-        <v>46200000000</v>
-      </c>
-      <c r="H30">
-        <f t="shared" si="3"/>
-        <v>8829370.1336672809</v>
-      </c>
-      <c r="I30">
-        <f t="shared" si="4"/>
-        <v>-429370.1336672809</v>
-      </c>
-    </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B31" s="34">
-        <f t="shared" si="5"/>
-        <v>26</v>
-      </c>
-      <c r="C31" s="35">
-        <v>8400000</v>
-      </c>
-      <c r="D31" s="36">
-        <v>7475</v>
-      </c>
-      <c r="E31" s="35">
-        <f t="shared" si="0"/>
-        <v>8400000</v>
-      </c>
-      <c r="F31">
-        <f t="shared" si="1"/>
-        <v>55875625</v>
-      </c>
-      <c r="G31" s="25">
-        <f t="shared" si="2"/>
-        <v>62790000000</v>
-      </c>
-      <c r="H31">
-        <f t="shared" si="3"/>
-        <v>9328250.3725365624</v>
-      </c>
-      <c r="I31">
-        <f t="shared" si="4"/>
-        <v>-928250.37253656238</v>
-      </c>
-    </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B32" s="34">
-        <f>B31+1</f>
-        <v>27</v>
-      </c>
-      <c r="C32" s="35">
-        <v>8400000</v>
-      </c>
-      <c r="D32" s="36">
-        <v>7000</v>
-      </c>
-      <c r="E32" s="35">
-        <f t="shared" si="0"/>
-        <v>8400000</v>
-      </c>
-      <c r="F32">
-        <f t="shared" si="1"/>
-        <v>49000000</v>
-      </c>
-      <c r="G32" s="25">
-        <f t="shared" si="2"/>
-        <v>58800000000</v>
-      </c>
-      <c r="H32">
-        <f t="shared" si="3"/>
-        <v>9208266.5176186338</v>
-      </c>
-      <c r="I32">
-        <f t="shared" si="4"/>
-        <v>-808266.51761863381</v>
-      </c>
-    </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B33" s="34">
-        <f t="shared" si="5"/>
-        <v>28</v>
-      </c>
-      <c r="C33" s="35">
-        <v>8295000</v>
-      </c>
-      <c r="D33" s="36">
-        <v>4880</v>
-      </c>
-      <c r="E33" s="35">
-        <f t="shared" si="0"/>
-        <v>8295000</v>
-      </c>
-      <c r="F33">
-        <f t="shared" si="1"/>
-        <v>23814400</v>
-      </c>
-      <c r="G33" s="25">
-        <f t="shared" si="2"/>
-        <v>40479600000</v>
-      </c>
-      <c r="H33">
-        <f t="shared" si="3"/>
-        <v>8672759.6283007227</v>
-      </c>
-      <c r="I33">
-        <f t="shared" si="4"/>
-        <v>-377759.62830072269</v>
-      </c>
-    </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B34" s="34">
-        <f t="shared" si="5"/>
-        <v>29</v>
-      </c>
-      <c r="C34" s="35">
-        <v>8190000</v>
-      </c>
-      <c r="D34" s="36">
-        <v>5960</v>
-      </c>
-      <c r="E34" s="35">
-        <f t="shared" si="0"/>
-        <v>8190000</v>
-      </c>
-      <c r="F34">
-        <f t="shared" si="1"/>
-        <v>35521600</v>
-      </c>
-      <c r="G34" s="25">
-        <f t="shared" si="2"/>
-        <v>48812400000</v>
-      </c>
-      <c r="H34">
-        <f t="shared" si="3"/>
-        <v>8945565.0247456953</v>
-      </c>
-      <c r="I34">
-        <f t="shared" si="4"/>
-        <v>-755565.02474569529</v>
-      </c>
-    </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B35" s="34">
-        <f t="shared" si="5"/>
-        <v>30</v>
-      </c>
-      <c r="C35" s="35">
-        <v>8120000</v>
-      </c>
-      <c r="D35" s="36">
-        <v>6840</v>
-      </c>
-      <c r="E35" s="35">
-        <f t="shared" si="0"/>
-        <v>8120000</v>
-      </c>
-      <c r="F35">
-        <f t="shared" si="1"/>
-        <v>46785600</v>
-      </c>
-      <c r="G35" s="25">
-        <f t="shared" si="2"/>
-        <v>55540800000</v>
-      </c>
-      <c r="H35">
-        <f t="shared" si="3"/>
-        <v>9167850.90333049</v>
-      </c>
-      <c r="I35">
-        <f t="shared" si="4"/>
-        <v>-1047850.90333049</v>
-      </c>
-    </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B36" s="34">
-        <f t="shared" si="5"/>
-        <v>31</v>
-      </c>
-      <c r="C36" s="35">
-        <v>8080940</v>
-      </c>
-      <c r="D36" s="36">
-        <v>7000</v>
-      </c>
-      <c r="E36" s="35">
-        <f t="shared" si="0"/>
-        <v>8080940</v>
-      </c>
-      <c r="F36">
-        <f t="shared" si="1"/>
-        <v>49000000</v>
-      </c>
-      <c r="G36" s="25">
-        <f t="shared" si="2"/>
-        <v>56566580000</v>
-      </c>
-      <c r="H36">
-        <f t="shared" si="3"/>
-        <v>9208266.5176186338</v>
-      </c>
-      <c r="I36">
-        <f t="shared" si="4"/>
-        <v>-1127326.5176186338</v>
-      </c>
-    </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B37" s="34">
-        <f t="shared" si="5"/>
-        <v>32</v>
-      </c>
-      <c r="C37" s="35">
-        <v>8043000</v>
-      </c>
-      <c r="D37" s="36">
-        <v>7482</v>
-      </c>
-      <c r="E37" s="35">
-        <f t="shared" si="0"/>
-        <v>8043000</v>
-      </c>
-      <c r="F37">
-        <f t="shared" si="1"/>
-        <v>55980324</v>
-      </c>
-      <c r="G37" s="25">
-        <f t="shared" si="2"/>
-        <v>60177726000</v>
-      </c>
-      <c r="H37">
-        <f t="shared" si="3"/>
-        <v>9330018.555661669</v>
-      </c>
-      <c r="I37">
-        <f t="shared" si="4"/>
-        <v>-1287018.555661669</v>
-      </c>
-    </row>
-    <row r="38" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B38" s="34">
-        <f t="shared" si="5"/>
-        <v>33</v>
-      </c>
-      <c r="C38" s="35">
-        <v>7980000</v>
-      </c>
-      <c r="D38" s="36">
-        <v>9000</v>
-      </c>
-      <c r="E38" s="35">
-        <f t="shared" si="0"/>
-        <v>7980000</v>
-      </c>
-      <c r="F38">
-        <f t="shared" si="1"/>
-        <v>81000000</v>
-      </c>
-      <c r="G38" s="25">
-        <f t="shared" si="2"/>
-        <v>71820000000</v>
-      </c>
-      <c r="H38">
-        <f t="shared" si="3"/>
-        <v>9713461.6962204371</v>
-      </c>
-      <c r="I38">
-        <f t="shared" si="4"/>
-        <v>-1733461.6962204371</v>
-      </c>
-    </row>
-    <row r="39" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B39" s="39">
-        <f t="shared" si="5"/>
-        <v>34</v>
-      </c>
-      <c r="C39" s="40">
-        <v>7962500</v>
-      </c>
-      <c r="D39" s="41">
-        <v>6000</v>
-      </c>
-      <c r="E39" s="35">
-        <f t="shared" si="0"/>
-        <v>7962500</v>
-      </c>
       <c r="F39" s="27">
-        <f t="shared" si="1"/>
-        <v>36000000</v>
+        <v>-993168.92831773125</v>
       </c>
       <c r="G39" s="28">
-        <f t="shared" si="2"/>
-        <v>47775000000</v>
-      </c>
-      <c r="H39">
-        <f t="shared" si="3"/>
-        <v>8955668.9283177312</v>
-      </c>
-      <c r="I39">
-        <f t="shared" si="4"/>
-        <v>-993168.92831773125</v>
-      </c>
-    </row>
-    <row r="40" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B40" s="45" t="s">
-        <v>22</v>
-      </c>
-      <c r="C40" s="1">
-        <f>SUM(C6:C39)</f>
-        <v>312850440</v>
-      </c>
-      <c r="D40" s="1">
-        <f>SUM(D6:D39)</f>
-        <v>237087</v>
-      </c>
-      <c r="E40" s="1"/>
-      <c r="F40" s="1">
-        <f>SUM(F6:F39)</f>
-        <v>1709971999</v>
-      </c>
-      <c r="G40" s="1">
-        <f>SUM(G6:G39)</f>
-        <v>2195881856000</v>
-      </c>
-    </row>
-    <row r="41" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B41" s="45"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
-    </row>
-    <row r="42" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B42" s="45"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
+        <v>986384520175.79077</v>
+      </c>
+      <c r="H39" s="52"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A40" s="52"/>
+      <c r="B40" s="52"/>
+      <c r="C40" s="52"/>
+      <c r="D40" s="52"/>
+      <c r="E40" s="52"/>
+      <c r="F40" s="52"/>
+      <c r="G40" s="54"/>
+      <c r="H40" s="52"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A41" s="52"/>
+      <c r="B41" s="52"/>
+      <c r="C41" s="52"/>
+      <c r="D41" s="52"/>
+      <c r="E41" s="52"/>
+      <c r="F41" s="52"/>
+      <c r="G41" s="52"/>
+      <c r="H41" s="52"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A42" s="52"/>
+      <c r="B42" s="52"/>
+      <c r="C42" s="52"/>
+      <c r="D42" s="52"/>
+      <c r="E42" s="52"/>
+      <c r="F42" s="52"/>
+      <c r="G42" s="52"/>
+      <c r="H42" s="52"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A43" s="52"/>
+      <c r="B43" s="52"/>
+      <c r="C43" s="52"/>
+      <c r="D43" s="52"/>
+      <c r="E43" s="52"/>
+      <c r="F43" s="52"/>
+      <c r="G43" s="52"/>
+      <c r="H43" s="52"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A44" s="52"/>
+      <c r="B44" s="52"/>
+      <c r="C44" s="52"/>
+      <c r="D44" s="52"/>
+      <c r="E44" s="52"/>
+      <c r="F44" s="52"/>
+      <c r="G44" s="52"/>
+      <c r="H44" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>